<commit_message>
Fruta / hortaliza, semanal
</commit_message>
<xml_diff>
--- a/PrecioFrutaHortalizas/Consolidado/logica_diaria/subcojuntos/Fruta, Agrícola del Norte S.A. de Arica - Arándano (blue).xlsx
+++ b/PrecioFrutaHortalizas/Consolidado/logica_diaria/subcojuntos/Fruta, Agrícola del Norte S.A. de Arica - Arándano (blue).xlsx
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>44881</v>
+        <v>44874</v>
       </c>
       <c r="E2" t="n">
         <v>15</v>
@@ -520,20 +520,20 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Segunda</t>
+          <t>Primera</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="N2" t="n">
-        <v>11250</v>
+        <v>7500</v>
       </c>
       <c r="O2" t="n">
-        <v>11250</v>
+        <v>8000</v>
       </c>
       <c r="P2" t="n">
-        <v>11250</v>
+        <v>7750</v>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="S2" t="n">
-        <v>11250</v>
+        <v>7750</v>
       </c>
       <c r="T2" t="n">
         <v>1</v>
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>44874</v>
+        <v>44881</v>
       </c>
       <c r="E3" t="n">
         <v>15</v>
@@ -600,20 +600,20 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Primera</t>
+          <t>Segunda</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="N3" t="n">
-        <v>7500</v>
+        <v>11250</v>
       </c>
       <c r="O3" t="n">
-        <v>8000</v>
+        <v>11250</v>
       </c>
       <c r="P3" t="n">
-        <v>7750</v>
+        <v>11250</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="S3" t="n">
-        <v>7750</v>
+        <v>11250</v>
       </c>
       <c r="T3" t="n">
         <v>1</v>

</xml_diff>